<commit_message>
Prevent the hold date to be more than 2 years in the future.
</commit_message>
<xml_diff>
--- a/eva_sub_cli/etc/EVA_Submission_Example.xlsx
+++ b/eva_sub_cli/etc/EVA_Submission_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-sub-cli/eva_sub_cli/etc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7FA69FC-B04D-8A4E-982E-07765320415B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D963ED4-68D9-7747-8A63-D71BEB7F2456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="30240" windowHeight="18980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -346,9 +346,6 @@
     <t>Hold Date</t>
   </si>
   <si>
-    <t>Date to publicly release (if in the future). In the format: yyyy-mm-dd</t>
-  </si>
-  <si>
     <t>Collaborator(s)</t>
   </si>
   <si>
@@ -2009,6 +2006,9 @@
   </si>
   <si>
     <t>my_file.vcf</t>
+  </si>
+  <si>
+    <t>Date to publicly release (if in the future). In the format: yyyy-mm-dd. The hold date should not be later than 2 years from now.</t>
   </si>
 </sst>
 </file>
@@ -2594,8 +2594,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2609,31 +2619,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2910,8 +2910,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1025" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="69"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2920,10 +2920,10 @@
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:1025" s="5" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="68"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -2932,10 +2932,10 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:1025" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="69"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -2944,10 +2944,10 @@
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:1025" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="70"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -2956,10 +2956,10 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:1025" s="5" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="71"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -4009,8 +4009,8 @@
       <c r="AMK7" s="5"/>
     </row>
     <row r="8" spans="1:1025" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="67"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -5036,10 +5036,10 @@
       <c r="AMK8" s="5"/>
     </row>
     <row r="9" spans="1:1025" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="70"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -6065,8 +6065,8 @@
       <c r="AMK9" s="5"/>
     </row>
     <row r="10" spans="1:1025" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="69"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -7092,10 +7092,10 @@
       <c r="AMK10" s="5"/>
     </row>
     <row r="11" spans="1:1025" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="74"/>
+      <c r="B11" s="71"/>
     </row>
     <row r="12" spans="1:1025" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
@@ -7147,10 +7147,10 @@
       </c>
     </row>
     <row r="19" spans="1:1025" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="72"/>
+      <c r="B19" s="68"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
@@ -8176,22 +8176,22 @@
       <c r="AMK19"/>
     </row>
     <row r="20" spans="1:1025" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="72"/>
+      <c r="B20" s="68"/>
     </row>
     <row r="21" spans="1:1025" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="72" t="s">
+      <c r="A21" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="72"/>
+      <c r="B21" s="68"/>
     </row>
     <row r="22" spans="1:1025" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="72"/>
+      <c r="B22" s="68"/>
     </row>
     <row r="23" spans="1:1025" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
@@ -9223,6 +9223,11 @@
   </sheetData>
   <sheetProtection password="E50B" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
@@ -9231,11 +9236,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -9256,20 +9256,20 @@
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -9317,7 +9317,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -9329,1645 +9329,1645 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
         <v>199</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>200</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>201</v>
-      </c>
-      <c r="E3" t="s">
-        <v>202</v>
       </c>
       <c r="F3" s="65"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
         <v>203</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>204</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>205</v>
-      </c>
-      <c r="E4" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" t="s">
         <v>207</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>208</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>209</v>
-      </c>
-      <c r="E5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" t="s">
         <v>211</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>212</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>213</v>
-      </c>
-      <c r="E6" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
         <v>215</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>216</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>217</v>
-      </c>
-      <c r="E7" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
         <v>219</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>220</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>221</v>
-      </c>
-      <c r="E8" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
         <v>223</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>224</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>225</v>
-      </c>
-      <c r="E9" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B10" t="s">
         <v>227</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>228</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>229</v>
-      </c>
-      <c r="E10" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" t="s">
         <v>231</v>
       </c>
-      <c r="B11" t="s">
+      <c r="E11" t="s">
         <v>232</v>
-      </c>
-      <c r="E11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" t="s">
         <v>234</v>
       </c>
-      <c r="B12" t="s">
-        <v>235</v>
-      </c>
       <c r="E12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>235</v>
+      </c>
+      <c r="E13" t="s">
         <v>236</v>
-      </c>
-      <c r="E13" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" t="s">
         <v>238</v>
-      </c>
-      <c r="E14" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E15" t="s">
         <v>240</v>
-      </c>
-      <c r="E15" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>241</v>
+      </c>
+      <c r="E16" t="s">
         <v>242</v>
-      </c>
-      <c r="E16" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>243</v>
+      </c>
+      <c r="E17" t="s">
         <v>244</v>
-      </c>
-      <c r="E17" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E18" t="s">
         <v>246</v>
-      </c>
-      <c r="E18" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>247</v>
+      </c>
+      <c r="E19" t="s">
         <v>248</v>
-      </c>
-      <c r="E19" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>249</v>
+      </c>
+      <c r="E20" t="s">
         <v>250</v>
-      </c>
-      <c r="E20" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>251</v>
+      </c>
+      <c r="E21" t="s">
         <v>252</v>
-      </c>
-      <c r="E21" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E22" t="s">
         <v>254</v>
-      </c>
-      <c r="E22" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>255</v>
+      </c>
+      <c r="E23" t="s">
         <v>256</v>
-      </c>
-      <c r="E23" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E24" t="s">
         <v>258</v>
-      </c>
-      <c r="E24" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>259</v>
+      </c>
+      <c r="E25" t="s">
         <v>260</v>
-      </c>
-      <c r="E25" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>261</v>
+      </c>
+      <c r="E26" t="s">
         <v>262</v>
-      </c>
-      <c r="E26" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
+        <v>263</v>
+      </c>
+      <c r="E27" t="s">
         <v>264</v>
-      </c>
-      <c r="E27" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>265</v>
+      </c>
+      <c r="E28" t="s">
         <v>266</v>
-      </c>
-      <c r="E28" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
+        <v>267</v>
+      </c>
+      <c r="E29" t="s">
         <v>268</v>
-      </c>
-      <c r="E29" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" t="s">
         <v>270</v>
-      </c>
-      <c r="E30" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
+        <v>271</v>
+      </c>
+      <c r="E31" t="s">
         <v>272</v>
-      </c>
-      <c r="E31" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
+        <v>273</v>
+      </c>
+      <c r="E32" t="s">
         <v>274</v>
-      </c>
-      <c r="E32" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
+        <v>275</v>
+      </c>
+      <c r="E33" t="s">
         <v>276</v>
-      </c>
-      <c r="E33" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>277</v>
+      </c>
+      <c r="E34" t="s">
         <v>278</v>
-      </c>
-      <c r="E34" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
+        <v>279</v>
+      </c>
+      <c r="E35" t="s">
         <v>280</v>
-      </c>
-      <c r="E35" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
+        <v>281</v>
+      </c>
+      <c r="E36" t="s">
         <v>282</v>
-      </c>
-      <c r="E36" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>283</v>
+      </c>
+      <c r="E37" t="s">
         <v>284</v>
-      </c>
-      <c r="E37" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" t="s">
         <v>286</v>
-      </c>
-      <c r="E38" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" t="s">
         <v>288</v>
-      </c>
-      <c r="E39" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" t="s">
         <v>290</v>
-      </c>
-      <c r="E40" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
+        <v>291</v>
+      </c>
+      <c r="E41" t="s">
         <v>292</v>
-      </c>
-      <c r="E41" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
+        <v>293</v>
+      </c>
+      <c r="E42" t="s">
         <v>294</v>
-      </c>
-      <c r="E42" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
+        <v>295</v>
+      </c>
+      <c r="E43" t="s">
         <v>296</v>
-      </c>
-      <c r="E43" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
+        <v>297</v>
+      </c>
+      <c r="E44" t="s">
         <v>298</v>
-      </c>
-      <c r="E44" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" t="s">
         <v>300</v>
-      </c>
-      <c r="E45" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
+        <v>301</v>
+      </c>
+      <c r="E46" t="s">
         <v>302</v>
-      </c>
-      <c r="E46" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>303</v>
+      </c>
+      <c r="E47" t="s">
         <v>304</v>
-      </c>
-      <c r="E47" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
+        <v>305</v>
+      </c>
+      <c r="E48" t="s">
         <v>306</v>
-      </c>
-      <c r="E48" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
+        <v>307</v>
+      </c>
+      <c r="E49" t="s">
         <v>308</v>
-      </c>
-      <c r="E49" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
+        <v>309</v>
+      </c>
+      <c r="E50" t="s">
         <v>310</v>
-      </c>
-      <c r="E50" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
+        <v>311</v>
+      </c>
+      <c r="E51" t="s">
         <v>312</v>
-      </c>
-      <c r="E51" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
+        <v>313</v>
+      </c>
+      <c r="E52" t="s">
         <v>314</v>
-      </c>
-      <c r="E52" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
+        <v>315</v>
+      </c>
+      <c r="E53" t="s">
         <v>316</v>
-      </c>
-      <c r="E53" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E55" s="40"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B168" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B174" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B179" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B188" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B191" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B197" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B202" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B203" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B204" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B205" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B206" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B207" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B208" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B228" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B229" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B230" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B231" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B232" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B233" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B234" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B235" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B236" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B237" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B238" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B239" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B240" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B241" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="282" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B282" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B283" s="66" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B284" s="66" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="285" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B285" s="66" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="286" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B286" s="66" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -10995,7 +10995,7 @@
     <col min="6" max="6" width="54.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
@@ -11017,42 +11017,42 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2" t="s">
         <v>551</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="67" t="s">
         <v>552</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="D2" t="s">
         <v>553</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>554</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>555</v>
-      </c>
-      <c r="F2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B3" t="s">
         <v>557</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="67" t="s">
         <v>558</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="D3" t="s">
         <v>559</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>560</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>561</v>
-      </c>
-      <c r="F3" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -11069,7 +11069,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11185,27 +11187,27 @@
         <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>587</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
         <v>56</v>
-      </c>
-      <c r="B16" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>59</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection password="E50B" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ix+uPfq92mfjOksbe2Bjdv4zbj3SdQ13OpWKhAVb3urdJzlcWKqfRgw9RK+P6ztn/cXXGDXfzXhp/iiR768b9w==" saltValue="qshIZYpIlnjT9Uv4tPnbgg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -11215,9 +11217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11239,13 +11239,13 @@
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="C1" s="30" t="s">
         <v>61</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>62</v>
       </c>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
@@ -11254,27 +11254,27 @@
     </row>
     <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="76" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="77" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="75"/>
+      <c r="B3" s="76"/>
       <c r="C3" s="20" t="s">
         <v>37</v>
       </c>
@@ -11306,39 +11306,39 @@
         <v>54</v>
       </c>
       <c r="M3" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N3" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
+        <v>562</v>
+      </c>
+      <c r="D4" t="s">
         <v>563</v>
       </c>
-      <c r="D4" t="s">
-        <v>564</v>
-      </c>
       <c r="E4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F4">
         <v>9606</v>
       </c>
       <c r="G4" t="s">
+        <v>564</v>
+      </c>
+      <c r="K4" t="s">
         <v>565</v>
-      </c>
-      <c r="K4" t="s">
-        <v>566</v>
       </c>
       <c r="L4" s="29">
         <v>46458</v>
       </c>
       <c r="M4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="N4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2"/>
@@ -11348,12 +11348,12 @@
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C2:N2"/>
   </mergeCells>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="B1" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Private data" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" sqref="L1:L1003" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Private data" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd" sqref="L2" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -11369,6 +11369,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Private data" prompt="On which date can the data be released publicly. In the format yyyy-mm-dd. The date should not be later than 2 years from now." sqref="L3:L1003 L1" xr:uid="{A2E2E95E-A82F-334F-9699-5ACD21C5AE13}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11399,18 +11400,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -11418,87 +11419,87 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
         <v>69</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
         <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
         <v>81</v>
-      </c>
-      <c r="B11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
         <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
-      </c>
-      <c r="B13" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" t="s">
         <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -11506,15 +11507,15 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
         <v>90</v>
-      </c>
-      <c r="B16" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
@@ -11560,84 +11561,84 @@
   <sheetData>
     <row r="1" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N1" s="22" t="s">
         <v>52</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>568</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="C2" t="s">
         <v>569</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" t="s">
         <v>570</v>
       </c>
-      <c r="D2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>571</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I2" t="s">
         <v>572</v>
       </c>
-      <c r="G2" t="s">
-        <v>287</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>573</v>
       </c>
-      <c r="J2" t="s">
-        <v>574</v>
-      </c>
       <c r="K2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="L2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="M2" s="33">
         <v>45728</v>
@@ -11732,73 +11733,73 @@
     </row>
     <row r="2" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="36" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>96</v>
       </c>
       <c r="C5" s="37"/>
     </row>
     <row r="6" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>99</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="36" t="s">
         <v>103</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>105</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -11806,36 +11807,36 @@
         <v>39</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="36" t="s">
         <v>108</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="36" t="s">
         <v>110</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B17" s="36"/>
     </row>
@@ -11844,327 +11845,327 @@
         <v>42</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>116</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>118</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" s="36"/>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>121</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="36" t="s">
         <v>123</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B24" s="36" t="s">
         <v>125</v>
-      </c>
-      <c r="B24" s="36" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B25" s="36"/>
     </row>
     <row r="26" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="36" t="s">
         <v>128</v>
-      </c>
-      <c r="B26" s="36" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="36" t="s">
         <v>130</v>
-      </c>
-      <c r="B27" s="36" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="36" t="s">
         <v>132</v>
-      </c>
-      <c r="B28" s="36" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29" s="36" t="s">
         <v>134</v>
-      </c>
-      <c r="B29" s="36" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="36" t="s">
         <v>136</v>
-      </c>
-      <c r="B30" s="36" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="36"/>
     </row>
     <row r="32" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="36" t="s">
         <v>139</v>
-      </c>
-      <c r="B32" s="36" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="36" t="s">
         <v>141</v>
-      </c>
-      <c r="B33" s="36" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" s="36" t="s">
         <v>143</v>
-      </c>
-      <c r="B34" s="36" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B35" s="36"/>
     </row>
     <row r="36" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="36" t="s">
         <v>146</v>
-      </c>
-      <c r="B36" s="36" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="36" t="s">
         <v>148</v>
-      </c>
-      <c r="B37" s="36" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="36" t="s">
         <v>150</v>
-      </c>
-      <c r="B38" s="36" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="36" t="s">
         <v>152</v>
-      </c>
-      <c r="B39" s="36" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="36" t="s">
         <v>154</v>
-      </c>
-      <c r="B40" s="36" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>155</v>
+      </c>
+      <c r="B41" s="36" t="s">
         <v>156</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" s="36" t="s">
         <v>158</v>
-      </c>
-      <c r="B42" s="36" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="36" t="s">
         <v>160</v>
-      </c>
-      <c r="B43" s="36" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>161</v>
+      </c>
+      <c r="B44" s="36" t="s">
         <v>162</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="41" t="s">
         <v>164</v>
-      </c>
-      <c r="B45" s="41" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B46" s="36"/>
     </row>
     <row r="47" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="36" t="s">
         <v>167</v>
-      </c>
-      <c r="B47" s="36" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B48" s="36" t="s">
         <v>169</v>
-      </c>
-      <c r="B48" s="36" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B49" s="36" t="s">
         <v>171</v>
-      </c>
-      <c r="B49" s="36" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="36" t="s">
         <v>173</v>
-      </c>
-      <c r="B50" s="36" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>174</v>
+      </c>
+      <c r="B51" s="36" t="s">
         <v>175</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="36" t="s">
         <v>177</v>
-      </c>
-      <c r="B52" s="36" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>178</v>
+      </c>
+      <c r="B53" s="36" t="s">
         <v>179</v>
-      </c>
-      <c r="B53" s="36" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="36" t="s">
         <v>181</v>
-      </c>
-      <c r="B54" s="36" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>182</v>
+      </c>
+      <c r="B55" s="36" t="s">
         <v>183</v>
-      </c>
-      <c r="B55" s="36" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="36" t="s">
         <v>185</v>
-      </c>
-      <c r="B56" s="36" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B57" s="36"/>
     </row>
     <row r="58" spans="1:2" ht="24" x14ac:dyDescent="0.2">
       <c r="A58" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B58" s="36"/>
     </row>
     <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B59" s="36"/>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>189</v>
+      </c>
+      <c r="B60" s="36" t="s">
         <v>190</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -12207,20 +12208,20 @@
     <col min="46" max="46" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:46" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>193</v>
-      </c>
-      <c r="E1" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>194</v>
       </c>
       <c r="G1" s="44"/>
       <c r="H1" s="45"/>
@@ -12263,286 +12264,286 @@
       <c r="AS1" s="46"/>
       <c r="AT1" s="48"/>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="49"/>
       <c r="B2" s="50"/>
-      <c r="C2" s="75"/>
+      <c r="C2" s="76"/>
       <c r="D2" s="51"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="78" t="s">
+      <c r="E2" s="76"/>
+      <c r="F2" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="79" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79" t="s">
+        <v>144</v>
+      </c>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="79"/>
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="79"/>
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="79"/>
+      <c r="AN2" s="79"/>
+      <c r="AO2" s="79"/>
+      <c r="AP2" s="79"/>
+      <c r="AQ2" s="79"/>
+      <c r="AR2" s="79"/>
+      <c r="AS2" s="79"/>
+    </row>
+    <row r="3" spans="1:46" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="76"/>
+      <c r="F3" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78" t="s">
-        <v>138</v>
-      </c>
-      <c r="X2" s="78"/>
-      <c r="Y2" s="78"/>
-      <c r="Z2" s="78" t="s">
-        <v>145</v>
-      </c>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="78"/>
-      <c r="AG2" s="78"/>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="78"/>
-      <c r="AM2" s="78"/>
-      <c r="AN2" s="78"/>
-      <c r="AO2" s="78"/>
-      <c r="AP2" s="78"/>
-      <c r="AQ2" s="78"/>
-      <c r="AR2" s="78"/>
-      <c r="AS2" s="78"/>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
-      <c r="A3" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="54" t="s">
-        <v>103</v>
-      </c>
       <c r="G3" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H3" s="56" t="s">
         <v>39</v>
       </c>
       <c r="I3" s="56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J3" s="56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K3" s="57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L3" s="55" t="s">
         <v>42</v>
       </c>
       <c r="M3" s="55" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N3" s="57" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O3" s="56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P3" s="58" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q3" s="56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R3" s="59" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S3" s="56" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T3" s="56" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U3" s="56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V3" s="57" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W3" s="59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="X3" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Y3" s="57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z3" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AA3" s="60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AB3" s="55" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AC3" s="56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AD3" s="56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AE3" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF3" s="56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AG3" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AH3" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AI3" s="57" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AJ3" s="59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AK3" s="56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AL3" s="56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AM3" s="56" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AN3" s="56" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AO3" s="56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AP3" s="56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AQ3" s="56" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AR3" s="56" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AS3" s="57" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AT3" s="61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B4" t="s">
+        <v>574</v>
+      </c>
+      <c r="D4" t="s">
         <v>575</v>
-      </c>
-      <c r="D4" t="s">
-        <v>576</v>
       </c>
       <c r="M4" s="62"/>
       <c r="Y4" s="29"/>
     </row>
     <row r="5" spans="1:46" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B5" t="s">
+        <v>576</v>
+      </c>
+      <c r="F5" t="s">
         <v>577</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>578</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>579</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>580</v>
       </c>
-      <c r="I5" t="s">
-        <v>581</v>
-      </c>
       <c r="J5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L5">
         <v>9606</v>
       </c>
       <c r="M5" s="63" t="s">
+        <v>581</v>
+      </c>
+      <c r="N5" t="s">
         <v>582</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q5" t="s">
         <v>583</v>
-      </c>
-      <c r="P5" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>584</v>
       </c>
       <c r="Y5" s="29"/>
       <c r="Z5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AA5" s="33">
         <v>45689</v>
       </c>
       <c r="AB5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC5" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="M6" s="62"/>
       <c r="Y6" s="29"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" ht="16" x14ac:dyDescent="0.2">
       <c r="M7" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="E1:E3"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:N2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Z2:AI2"/>
     <mergeCell ref="AJ2:AS2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="E1:E3"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="L2:N2"/>
   </mergeCells>
   <dataValidations count="6">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="E1 B4:B1003" xr:uid="{00000000-0002-0000-0700-000000000000}">
@@ -12630,18 +12631,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" t="s">
         <v>196</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>